<commit_message>
added more price quotes from vendors. R6_bom_dk_ab_mous has the prices we got for everything.
</commit_message>
<xml_diff>
--- a/Circuit/R6/extended_r6_target_prices.xlsx
+++ b/Circuit/R6/extended_r6_target_prices.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="194">
   <si>
     <t>Item Number</t>
   </si>
@@ -583,6 +583,24 @@
   </si>
   <si>
     <t>Target Price(10qty)</t>
+  </si>
+  <si>
+    <t>quoted price (qty listed in column B)</t>
+  </si>
+  <si>
+    <t>Quoted price (10x qty listed in column b)</t>
+  </si>
+  <si>
+    <t>Reel qty</t>
+  </si>
+  <si>
+    <t>unit price for full reel</t>
+  </si>
+  <si>
+    <t>Vendor Name:</t>
+  </si>
+  <si>
+    <t>qty available for immediate shipping</t>
   </si>
 </sst>
 </file>
@@ -630,12 +648,49 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -645,7 +700,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -657,6 +712,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -946,446 +1009,447 @@
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" customWidth="1"/>
     <col min="7" max="7" width="25.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="18" style="6" customWidth="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A1" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
+      <c r="I2" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H3" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
+    <row r="4" spans="1:13">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>44</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>176</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H4" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>66</v>
+        <v>176</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>66</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H7" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H8" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H9" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H10" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H11" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H12" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H13" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H14" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
-        <v>11</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16" s="1">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H16" s="4">
         <v>0.31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="H17" s="5">
         <v>0.4</v>
@@ -1393,129 +1457,129 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="4">
-        <v>8.3000000000000004E-2</v>
+        <v>58</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0.15</v>
+        <v>63</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="4">
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>11</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H20" s="5">
-        <v>3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="H21" s="5">
-        <v>0.1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>11</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>79</v>
+      <c r="G22" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="H22" s="5">
         <v>0.1</v>
@@ -1523,25 +1587,25 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H23" s="5">
         <v>0.1</v>
@@ -1549,25 +1613,25 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H24" s="5">
         <v>0.1</v>
@@ -1575,129 +1639,129 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>87</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H25" s="4">
-        <v>0.245</v>
+        <v>88</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H26" s="5">
-        <v>1.9</v>
+        <v>91</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.245</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>11</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H27" s="5">
-        <v>0</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H28" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H29" s="5">
         <v>0.01</v>
@@ -1705,25 +1769,25 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H30" s="5">
         <v>0.01</v>
@@ -1731,25 +1795,25 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H31" s="5">
         <v>0.01</v>
@@ -1757,25 +1821,25 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H32" s="5">
         <v>0.01</v>
@@ -1783,25 +1847,25 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>11</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H33" s="5">
         <v>0.01</v>
@@ -1809,25 +1873,25 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>11</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H34" s="5">
         <v>0.01</v>
@@ -1835,25 +1899,25 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>11</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H35" s="5">
         <v>0.01</v>
@@ -1861,25 +1925,25 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>11</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H36" s="5">
         <v>0.01</v>
@@ -1887,25 +1951,25 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>11</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H37" s="5">
         <v>0.01</v>
@@ -1913,25 +1977,25 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>11</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H38" s="5">
         <v>0.01</v>
@@ -1939,25 +2003,25 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>11</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>102</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H39" s="5">
         <v>0.01</v>
@@ -1965,77 +2029,77 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>11</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H40" s="4">
-        <v>0.68700000000000006</v>
+        <v>136</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0.01</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1">
         <v>11</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H41" s="5">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0.68700000000000006</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>11</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H42" s="5">
         <v>1</v>
@@ -2043,291 +2107,320 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1">
         <v>11</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H43" s="5">
-        <v>2.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1">
         <v>11</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H44" s="5">
-        <v>1.35</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1">
         <v>11</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H45" s="4">
-        <v>2.016</v>
+        <v>153</v>
+      </c>
+      <c r="H45" s="5">
+        <v>1.35</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1">
         <v>11</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>156</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H46" s="4">
-        <v>9</v>
+        <v>2.016</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1">
         <v>11</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H47" s="5">
-        <v>2.2000000000000002</v>
+        <v>158</v>
+      </c>
+      <c r="H47" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1">
         <v>11</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H48" s="5">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1">
         <v>11</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H49" s="5">
-        <v>0.36</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1">
         <v>11</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="H50" s="5">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="1">
         <v>11</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="H51" s="5">
-        <v>1.6950000000000001</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1">
         <v>11</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>177</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H52" s="5">
-        <v>0.5</v>
+        <v>1.6950000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1">
+        <v>54</v>
+      </c>
+      <c r="B53" s="1">
+        <v>11</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H53" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1">
         <v>55</v>
       </c>
-      <c r="B53" s="1">
-        <v>11</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="B54" s="1">
+        <v>11</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="H53" s="5">
+      <c r="H54" s="5">
         <v>0.6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>